<commit_message>
replaced blk text with blue
</commit_message>
<xml_diff>
--- a/static/documents/Supplemental_data.xlsx
+++ b/static/documents/Supplemental_data.xlsx
@@ -1,37 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blucci\Desktop\piv\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413CFDD5-DD2F-480A-AD68-C5873B926B7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14556" windowHeight="7812" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestChart" sheetId="11" r:id="rId1"/>
     <sheet name="All Data" sheetId="8" r:id="rId2"/>
     <sheet name="Array Descriptions" sheetId="7" r:id="rId3"/>
     <sheet name="SmoothEndwallLimits" sheetId="12" r:id="rId4"/>
+    <sheet name="GeometryParameters" sheetId="13" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="diary." localSheetId="2">'Array Descriptions'!$A$1:$C$37</definedName>
   </definedNames>
-  <calcPr calcId="162913" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="191029" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="diary" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="diary" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr sourceFile="C:\Users\blucci\Documents\MATLAB\diary." delimited="0">
       <textFields count="3">
         <textField/>
@@ -2171,7 +2179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3389,46 +3397,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3440,10 +3421,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3479,55 +3496,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -6771,7 +6779,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6809,7 +6823,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6853,7 +6873,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6891,7 +6917,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6929,7 +6961,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6955,8 +6993,57 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57072</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59EA1B0-10CC-4A91-A5FC-BB5DDE3B6793}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="182880"/>
+          <a:ext cx="4693920" cy="2983152"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="diary." connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="diary." connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7221,10 +7308,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:P70"/>
   <sheetViews>
-    <sheetView topLeftCell="D46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -7256,51 +7343,51 @@
       <c r="D4" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="75" t="s">
         <v>398</v>
       </c>
-      <c r="F4" s="121"/>
+      <c r="F4" s="76"/>
       <c r="G4" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="H4" s="120" t="s">
+      <c r="H4" s="75" t="s">
         <v>400</v>
       </c>
-      <c r="I4" s="121"/>
+      <c r="I4" s="76"/>
       <c r="J4" s="12" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="5" spans="4:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="108" t="s">
+      <c r="D5" s="77" t="s">
         <v>402</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="79" t="s">
         <v>403</v>
       </c>
-      <c r="F5" s="89"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="63">
         <v>0.25</v>
       </c>
-      <c r="H5" s="110" t="s">
+      <c r="H5" s="83" t="s">
         <v>404</v>
       </c>
-      <c r="I5" s="111"/>
+      <c r="I5" s="84"/>
       <c r="J5" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="109"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="91"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="64">
         <v>0.35</v>
       </c>
-      <c r="H6" s="112" t="s">
+      <c r="H6" s="85" t="s">
         <v>404</v>
       </c>
-      <c r="I6" s="113"/>
+      <c r="I6" s="86"/>
       <c r="J6" s="14">
         <v>6</v>
       </c>
@@ -7315,35 +7402,35 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D8" s="108" t="s">
+      <c r="D8" s="77" t="s">
         <v>405</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="79" t="s">
         <v>403</v>
       </c>
-      <c r="F8" s="89"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="63">
         <v>0.25</v>
       </c>
-      <c r="H8" s="110" t="s">
+      <c r="H8" s="83" t="s">
         <v>404</v>
       </c>
-      <c r="I8" s="111"/>
+      <c r="I8" s="84"/>
       <c r="J8" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="109"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="82"/>
       <c r="G9" s="64">
         <v>0.35</v>
       </c>
-      <c r="H9" s="112" t="s">
+      <c r="H9" s="85" t="s">
         <v>404</v>
       </c>
-      <c r="I9" s="113"/>
+      <c r="I9" s="86"/>
       <c r="J9" s="14">
         <v>14</v>
       </c>
@@ -7358,10 +7445,10 @@
       <c r="J10" s="19"/>
     </row>
     <row r="11" spans="4:16" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="87" t="s">
         <v>406</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="91" t="s">
         <v>403</v>
       </c>
       <c r="F11" s="67" t="s">
@@ -7382,8 +7469,8 @@
       <c r="K11" s="23"/>
     </row>
     <row r="12" spans="4:16" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="115"/>
-      <c r="E12" s="76"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="89"/>
       <c r="F12" s="24"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -7391,9 +7478,9 @@
       <c r="J12" s="25"/>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="75" t="s">
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="91" t="s">
         <v>409</v>
       </c>
       <c r="G13" s="26">
@@ -7410,64 +7497,64 @@
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D14" s="115"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="117">
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="93">
         <v>0.35</v>
       </c>
       <c r="H14" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="I14" s="118" t="s">
+      <c r="I14" s="94" t="s">
         <v>404</v>
       </c>
-      <c r="J14" s="94">
+      <c r="J14" s="97">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D15" s="115"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="117"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="93"/>
       <c r="H15" s="65" t="s">
         <v>410</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="98"/>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="96">
+      <c r="D16" s="88"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="99">
         <v>0.38</v>
       </c>
       <c r="H16" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="I16" s="98" t="s">
+      <c r="I16" s="101" t="s">
         <v>404</v>
       </c>
-      <c r="J16" s="100">
+      <c r="J16" s="103">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="97"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="100"/>
       <c r="H17" s="60" t="s">
         <v>410</v>
       </c>
-      <c r="I17" s="99"/>
-      <c r="J17" s="101"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="104"/>
     </row>
     <row r="18" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="115"/>
-      <c r="E18" s="76"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="89"/>
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
@@ -7475,8 +7562,8 @@
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="115"/>
-      <c r="E19" s="78"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="92"/>
       <c r="F19" s="33" t="s">
         <v>411</v>
       </c>
@@ -7494,7 +7581,7 @@
       </c>
     </row>
     <row r="20" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="76"/>
+      <c r="D20" s="89"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -7503,57 +7590,57 @@
       <c r="J20" s="29"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D21" s="115"/>
-      <c r="E21" s="75" t="s">
+      <c r="D21" s="88"/>
+      <c r="E21" s="91" t="s">
         <v>412</v>
       </c>
-      <c r="F21" s="102" t="s">
+      <c r="F21" s="105" t="s">
         <v>413</v>
       </c>
       <c r="G21" s="26">
         <v>0.25</v>
       </c>
-      <c r="H21" s="105" t="s">
+      <c r="H21" s="96" t="s">
         <v>414</v>
       </c>
-      <c r="I21" s="105"/>
+      <c r="I21" s="96"/>
       <c r="J21" s="28">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D22" s="115"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="103"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="58">
         <v>0.35</v>
       </c>
-      <c r="H22" s="106" t="s">
+      <c r="H22" s="108" t="s">
         <v>414</v>
       </c>
-      <c r="I22" s="106"/>
+      <c r="I22" s="108"/>
       <c r="J22" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="115"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="104"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="107"/>
       <c r="G23" s="71">
         <v>0.38</v>
       </c>
-      <c r="H23" s="107" t="s">
+      <c r="H23" s="109" t="s">
         <v>414</v>
       </c>
-      <c r="I23" s="107"/>
+      <c r="I23" s="109"/>
       <c r="J23" s="38">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="115"/>
-      <c r="E24" s="76"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="89"/>
       <c r="F24" s="39"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
@@ -7561,33 +7648,33 @@
       <c r="J24" s="40"/>
     </row>
     <row r="25" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="115"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="102" t="s">
+      <c r="D25" s="88"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="105" t="s">
         <v>415</v>
       </c>
       <c r="G25" s="26">
         <v>0.35</v>
       </c>
-      <c r="H25" s="105" t="s">
+      <c r="H25" s="96" t="s">
         <v>414</v>
       </c>
-      <c r="I25" s="105"/>
+      <c r="I25" s="96"/>
       <c r="J25" s="28">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="116"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="104"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="107"/>
       <c r="G26" s="71">
         <v>0.38</v>
       </c>
-      <c r="H26" s="107" t="s">
+      <c r="H26" s="109" t="s">
         <v>414</v>
       </c>
-      <c r="I26" s="107"/>
+      <c r="I26" s="109"/>
       <c r="J26" s="38">
         <v>14</v>
       </c>
@@ -7602,55 +7689,55 @@
       <c r="J27" s="16"/>
     </row>
     <row r="28" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="75" t="s">
+      <c r="D28" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="E28" s="75" t="s">
+      <c r="E28" s="91" t="s">
         <v>417</v>
       </c>
-      <c r="F28" s="79" t="s">
+      <c r="F28" s="111" t="s">
         <v>418</v>
       </c>
       <c r="G28" s="62">
         <v>0.25</v>
       </c>
-      <c r="H28" s="81" t="s">
+      <c r="H28" s="79" t="s">
         <v>414</v>
       </c>
-      <c r="I28" s="82"/>
+      <c r="I28" s="113"/>
       <c r="J28" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="77"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="110"/>
       <c r="G29" s="43">
         <v>0.35</v>
       </c>
-      <c r="H29" s="83"/>
-      <c r="I29" s="84"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="115"/>
       <c r="J29" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="80"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="112"/>
       <c r="G30" s="61">
         <v>0.38</v>
       </c>
-      <c r="H30" s="85"/>
-      <c r="I30" s="86"/>
+      <c r="H30" s="116"/>
+      <c r="I30" s="117"/>
       <c r="J30" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="76"/>
-      <c r="E31" s="77"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="110"/>
       <c r="F31" s="47"/>
       <c r="G31" s="48"/>
       <c r="H31" s="48"/>
@@ -7658,50 +7745,50 @@
       <c r="J31" s="49"/>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="79" t="s">
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="111" t="s">
         <v>415</v>
       </c>
       <c r="G32" s="62">
         <v>0.25</v>
       </c>
-      <c r="H32" s="81" t="s">
+      <c r="H32" s="79" t="s">
         <v>419</v>
       </c>
-      <c r="I32" s="82"/>
+      <c r="I32" s="113"/>
       <c r="J32" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="77"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="110"/>
       <c r="G33" s="43">
         <v>0.35</v>
       </c>
-      <c r="H33" s="83"/>
-      <c r="I33" s="84"/>
+      <c r="H33" s="114"/>
+      <c r="I33" s="115"/>
       <c r="J33" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="76"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="80"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="112"/>
       <c r="G34" s="61">
         <v>0.38</v>
       </c>
-      <c r="H34" s="85"/>
-      <c r="I34" s="86"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="117"/>
       <c r="J34" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D35" s="77"/>
+      <c r="D35" s="110"/>
       <c r="E35" s="47"/>
       <c r="F35" s="47"/>
       <c r="G35" s="48"/>
@@ -7710,53 +7797,53 @@
       <c r="J35" s="49"/>
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D36" s="76"/>
-      <c r="E36" s="75" t="s">
+      <c r="D36" s="89"/>
+      <c r="E36" s="91" t="s">
         <v>420</v>
       </c>
-      <c r="F36" s="79" t="s">
+      <c r="F36" s="111" t="s">
         <v>421</v>
       </c>
       <c r="G36" s="62">
         <v>0.25</v>
       </c>
-      <c r="H36" s="81" t="s">
+      <c r="H36" s="79" t="s">
         <v>404</v>
       </c>
-      <c r="I36" s="82"/>
+      <c r="I36" s="113"/>
       <c r="J36" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="77"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="110"/>
       <c r="G37" s="43">
         <v>0.35</v>
       </c>
-      <c r="H37" s="83"/>
-      <c r="I37" s="84"/>
+      <c r="H37" s="114"/>
+      <c r="I37" s="115"/>
       <c r="J37" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="80"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="112"/>
       <c r="G38" s="61">
         <v>0.38</v>
       </c>
-      <c r="H38" s="85"/>
-      <c r="I38" s="86"/>
+      <c r="H38" s="116"/>
+      <c r="I38" s="117"/>
       <c r="J38" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="76"/>
-      <c r="E39" s="77"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="110"/>
       <c r="F39" s="47"/>
       <c r="G39" s="48"/>
       <c r="H39" s="48"/>
@@ -7764,51 +7851,51 @@
       <c r="J39" s="49"/>
     </row>
     <row r="40" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="79" t="s">
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="111" t="s">
         <v>422</v>
       </c>
       <c r="G40" s="62">
         <v>0.25</v>
       </c>
-      <c r="H40" s="81" t="s">
+      <c r="H40" s="79" t="s">
         <v>404</v>
       </c>
-      <c r="I40" s="82"/>
+      <c r="I40" s="113"/>
       <c r="J40" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="77"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="110"/>
       <c r="G41" s="43">
         <v>0.35</v>
       </c>
-      <c r="H41" s="83"/>
-      <c r="I41" s="84"/>
+      <c r="H41" s="114"/>
+      <c r="I41" s="115"/>
       <c r="J41" s="44">
         <v>14</v>
       </c>
       <c r="O41" s="50"/>
     </row>
     <row r="42" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="76"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="80"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="112"/>
       <c r="G42" s="61">
         <v>0.38</v>
       </c>
-      <c r="H42" s="85"/>
-      <c r="I42" s="86"/>
+      <c r="H42" s="116"/>
+      <c r="I42" s="117"/>
       <c r="J42" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D43" s="77"/>
+      <c r="D43" s="110"/>
       <c r="E43" s="47"/>
       <c r="F43" s="47"/>
       <c r="G43" s="48"/>
@@ -7817,33 +7904,33 @@
       <c r="J43" s="49"/>
     </row>
     <row r="44" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D44" s="76"/>
-      <c r="E44" s="79" t="s">
+      <c r="D44" s="89"/>
+      <c r="E44" s="111" t="s">
         <v>423</v>
       </c>
-      <c r="F44" s="87" t="s">
+      <c r="F44" s="118" t="s">
         <v>424</v>
       </c>
       <c r="G44" s="41">
         <v>0.25</v>
       </c>
-      <c r="H44" s="81" t="s">
+      <c r="H44" s="79" t="s">
         <v>425</v>
       </c>
-      <c r="I44" s="89"/>
+      <c r="I44" s="80"/>
       <c r="J44" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D45" s="78"/>
-      <c r="E45" s="80"/>
-      <c r="F45" s="88"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="119"/>
       <c r="G45" s="45">
         <v>0.38</v>
       </c>
-      <c r="H45" s="90"/>
-      <c r="I45" s="91"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="82"/>
       <c r="J45" s="46">
         <v>1</v>
       </c>
@@ -7858,55 +7945,55 @@
       <c r="J46" s="53"/>
     </row>
     <row r="47" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="75" t="s">
+      <c r="D47" s="91" t="s">
         <v>426</v>
       </c>
-      <c r="E47" s="75" t="s">
+      <c r="E47" s="91" t="s">
         <v>417</v>
       </c>
-      <c r="F47" s="79" t="s">
+      <c r="F47" s="111" t="s">
         <v>418</v>
       </c>
       <c r="G47" s="62">
         <v>0.25</v>
       </c>
-      <c r="H47" s="81" t="s">
+      <c r="H47" s="79" t="s">
         <v>419</v>
       </c>
-      <c r="I47" s="82"/>
+      <c r="I47" s="113"/>
       <c r="J47" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="48" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D48" s="76"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="77"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="89"/>
+      <c r="F48" s="110"/>
       <c r="G48" s="43">
         <v>0.35</v>
       </c>
-      <c r="H48" s="83"/>
-      <c r="I48" s="84"/>
+      <c r="H48" s="114"/>
+      <c r="I48" s="115"/>
       <c r="J48" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="76"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="80"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="112"/>
       <c r="G49" s="61">
         <v>0.38</v>
       </c>
-      <c r="H49" s="85"/>
-      <c r="I49" s="86"/>
+      <c r="H49" s="116"/>
+      <c r="I49" s="117"/>
       <c r="J49" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D50" s="76"/>
-      <c r="E50" s="77"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="110"/>
       <c r="F50" s="47"/>
       <c r="G50" s="48"/>
       <c r="H50" s="48"/>
@@ -7914,50 +8001,50 @@
       <c r="J50" s="49"/>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D51" s="76"/>
-      <c r="E51" s="76"/>
-      <c r="F51" s="79" t="s">
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="111" t="s">
         <v>415</v>
       </c>
       <c r="G51" s="62">
         <v>0.25</v>
       </c>
-      <c r="H51" s="81" t="s">
+      <c r="H51" s="79" t="s">
         <v>419</v>
       </c>
-      <c r="I51" s="82"/>
+      <c r="I51" s="113"/>
       <c r="J51" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D52" s="76"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="77"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="110"/>
       <c r="G52" s="43">
         <v>0.35</v>
       </c>
-      <c r="H52" s="83"/>
-      <c r="I52" s="84"/>
+      <c r="H52" s="114"/>
+      <c r="I52" s="115"/>
       <c r="J52" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D53" s="76"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="80"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="92"/>
+      <c r="F53" s="112"/>
       <c r="G53" s="61">
         <v>0.38</v>
       </c>
-      <c r="H53" s="85"/>
-      <c r="I53" s="86"/>
+      <c r="H53" s="116"/>
+      <c r="I53" s="117"/>
       <c r="J53" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="54" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="77"/>
+      <c r="D54" s="110"/>
       <c r="E54" s="47"/>
       <c r="F54" s="47"/>
       <c r="G54" s="48"/>
@@ -7966,53 +8053,53 @@
       <c r="J54" s="49"/>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D55" s="76"/>
-      <c r="E55" s="75" t="s">
+      <c r="D55" s="89"/>
+      <c r="E55" s="91" t="s">
         <v>420</v>
       </c>
-      <c r="F55" s="79" t="s">
+      <c r="F55" s="111" t="s">
         <v>421</v>
       </c>
       <c r="G55" s="62">
         <v>0.25</v>
       </c>
-      <c r="H55" s="81" t="s">
+      <c r="H55" s="79" t="s">
         <v>404</v>
       </c>
-      <c r="I55" s="89"/>
+      <c r="I55" s="80"/>
       <c r="J55" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D56" s="76"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="77"/>
+      <c r="D56" s="89"/>
+      <c r="E56" s="89"/>
+      <c r="F56" s="110"/>
       <c r="G56" s="43">
         <v>0.35</v>
       </c>
-      <c r="H56" s="92"/>
-      <c r="I56" s="93"/>
+      <c r="H56" s="120"/>
+      <c r="I56" s="121"/>
       <c r="J56" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="57" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D57" s="76"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="80"/>
+      <c r="D57" s="89"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="112"/>
       <c r="G57" s="61">
         <v>0.38</v>
       </c>
-      <c r="H57" s="90"/>
-      <c r="I57" s="91"/>
+      <c r="H57" s="81"/>
+      <c r="I57" s="82"/>
       <c r="J57" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="58" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D58" s="76"/>
-      <c r="E58" s="77"/>
+      <c r="D58" s="89"/>
+      <c r="E58" s="110"/>
       <c r="F58" s="47"/>
       <c r="G58" s="48"/>
       <c r="H58" s="48"/>
@@ -8020,50 +8107,50 @@
       <c r="J58" s="49"/>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D59" s="76"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="79" t="s">
+      <c r="D59" s="89"/>
+      <c r="E59" s="89"/>
+      <c r="F59" s="111" t="s">
         <v>427</v>
       </c>
       <c r="G59" s="62">
         <v>0.25</v>
       </c>
-      <c r="H59" s="81" t="s">
+      <c r="H59" s="79" t="s">
         <v>404</v>
       </c>
-      <c r="I59" s="89"/>
+      <c r="I59" s="80"/>
       <c r="J59" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D60" s="76"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="77"/>
+      <c r="D60" s="89"/>
+      <c r="E60" s="89"/>
+      <c r="F60" s="110"/>
       <c r="G60" s="43">
         <v>0.35</v>
       </c>
-      <c r="H60" s="92"/>
-      <c r="I60" s="93"/>
+      <c r="H60" s="120"/>
+      <c r="I60" s="121"/>
       <c r="J60" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D61" s="76"/>
-      <c r="E61" s="78"/>
-      <c r="F61" s="80"/>
+      <c r="D61" s="89"/>
+      <c r="E61" s="92"/>
+      <c r="F61" s="112"/>
       <c r="G61" s="61">
         <v>0.38</v>
       </c>
-      <c r="H61" s="90"/>
-      <c r="I61" s="91"/>
+      <c r="H61" s="81"/>
+      <c r="I61" s="82"/>
       <c r="J61" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="62" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D62" s="76"/>
+      <c r="D62" s="89"/>
       <c r="E62" s="54"/>
       <c r="F62" s="47"/>
       <c r="G62" s="48"/>
@@ -8072,33 +8159,33 @@
       <c r="J62" s="49"/>
     </row>
     <row r="63" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D63" s="76"/>
-      <c r="E63" s="79" t="s">
+      <c r="D63" s="89"/>
+      <c r="E63" s="111" t="s">
         <v>423</v>
       </c>
-      <c r="F63" s="87" t="s">
+      <c r="F63" s="118" t="s">
         <v>424</v>
       </c>
       <c r="G63" s="62">
         <v>0.25</v>
       </c>
-      <c r="H63" s="81" t="s">
+      <c r="H63" s="79" t="s">
         <v>425</v>
       </c>
-      <c r="I63" s="89"/>
+      <c r="I63" s="80"/>
       <c r="J63" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D64" s="78"/>
-      <c r="E64" s="80"/>
-      <c r="F64" s="88"/>
+      <c r="D64" s="92"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="119"/>
       <c r="G64" s="61">
         <v>0.38</v>
       </c>
-      <c r="H64" s="90"/>
-      <c r="I64" s="91"/>
+      <c r="H64" s="81"/>
+      <c r="I64" s="82"/>
       <c r="J64" s="46">
         <v>1</v>
       </c>
@@ -8120,33 +8207,20 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D11:D26"/>
-    <mergeCell ref="E11:E19"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D47:D64"/>
+    <mergeCell ref="E47:E53"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="H47:I49"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="H63:I64"/>
+    <mergeCell ref="H51:I53"/>
+    <mergeCell ref="E55:E61"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="H55:I57"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="H59:I61"/>
     <mergeCell ref="D28:D45"/>
     <mergeCell ref="E28:E34"/>
     <mergeCell ref="F28:F30"/>
@@ -8161,20 +8235,33 @@
     <mergeCell ref="E44:E45"/>
     <mergeCell ref="F44:F45"/>
     <mergeCell ref="H44:I45"/>
-    <mergeCell ref="D47:D64"/>
-    <mergeCell ref="E47:E53"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="H47:I49"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="H63:I64"/>
-    <mergeCell ref="H51:I53"/>
-    <mergeCell ref="E55:E61"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="H55:I57"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="H59:I61"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D11:D26"/>
+    <mergeCell ref="E11:E19"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8183,10 +8270,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G447"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G236" sqref="G236"/>
     </sheetView>
   </sheetViews>
@@ -11844,7 +11931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12228,7 +12315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12729,4 +12816,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49005765-97C5-4AC1-AFAA-5931329AAD44}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Normalizing parameters to supplemental data file
</commit_message>
<xml_diff>
--- a/static/documents/Supplemental_data.xlsx
+++ b/static/documents/Supplemental_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blucci\Desktop\piv\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413CFDD5-DD2F-480A-AD68-C5873B926B7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6273F7F-3EEA-4E6C-B8A2-2DC3485A6647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="3192" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestChart" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="503">
   <si>
     <t>Q25_smooth_small_sc655</t>
   </si>
@@ -2175,12 +2177,27 @@
   <si>
     <t>Gap size is 1.8 mm. with casing treatment</t>
   </si>
+  <si>
+    <t>normvor = 1000./(2*pi*8)</t>
+  </si>
+  <si>
+    <t>normTKE = 1./(11.4*11.4)</t>
+  </si>
+  <si>
+    <t>normvel = 1/11.47</t>
+  </si>
+  <si>
+    <t>Normalizing Parameter (multiply by:)</t>
+  </si>
+  <si>
+    <t>normprod = 1./normvel.^2.*normvor/1000.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2330,6 +2347,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -2381,7 +2404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="65">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -3203,11 +3226,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3397,19 +3429,46 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3421,46 +3480,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3496,48 +3519,60 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7311,7 +7346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -7343,51 +7378,51 @@
       <c r="D4" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="120" t="s">
         <v>398</v>
       </c>
-      <c r="F4" s="76"/>
+      <c r="F4" s="121"/>
       <c r="G4" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="120" t="s">
         <v>400</v>
       </c>
-      <c r="I4" s="76"/>
+      <c r="I4" s="121"/>
       <c r="J4" s="12" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="5" spans="4:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="108" t="s">
         <v>402</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="81" t="s">
         <v>403</v>
       </c>
-      <c r="F5" s="80"/>
+      <c r="F5" s="89"/>
       <c r="G5" s="63">
         <v>0.25</v>
       </c>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="110" t="s">
         <v>404</v>
       </c>
-      <c r="I5" s="84"/>
+      <c r="I5" s="111"/>
       <c r="J5" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="78"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="82"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="91"/>
       <c r="G6" s="64">
         <v>0.35</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="112" t="s">
         <v>404</v>
       </c>
-      <c r="I6" s="86"/>
+      <c r="I6" s="113"/>
       <c r="J6" s="14">
         <v>6</v>
       </c>
@@ -7402,35 +7437,35 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="108" t="s">
         <v>405</v>
       </c>
-      <c r="E8" s="79" t="s">
+      <c r="E8" s="81" t="s">
         <v>403</v>
       </c>
-      <c r="F8" s="80"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="63">
         <v>0.25</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="110" t="s">
         <v>404</v>
       </c>
-      <c r="I8" s="84"/>
+      <c r="I8" s="111"/>
       <c r="J8" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="78"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="82"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="91"/>
       <c r="G9" s="64">
         <v>0.35</v>
       </c>
-      <c r="H9" s="85" t="s">
+      <c r="H9" s="112" t="s">
         <v>404</v>
       </c>
-      <c r="I9" s="86"/>
+      <c r="I9" s="113"/>
       <c r="J9" s="14">
         <v>14</v>
       </c>
@@ -7445,10 +7480,10 @@
       <c r="J10" s="19"/>
     </row>
     <row r="11" spans="4:16" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="114" t="s">
         <v>406</v>
       </c>
-      <c r="E11" s="91" t="s">
+      <c r="E11" s="75" t="s">
         <v>403</v>
       </c>
       <c r="F11" s="67" t="s">
@@ -7469,8 +7504,8 @@
       <c r="K11" s="23"/>
     </row>
     <row r="12" spans="4:16" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="88"/>
-      <c r="E12" s="89"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="76"/>
       <c r="F12" s="24"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -7478,9 +7513,9 @@
       <c r="J12" s="25"/>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="91" t="s">
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="75" t="s">
         <v>409</v>
       </c>
       <c r="G13" s="26">
@@ -7497,64 +7532,64 @@
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="93">
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="117">
         <v>0.35</v>
       </c>
       <c r="H14" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="I14" s="94" t="s">
+      <c r="I14" s="118" t="s">
         <v>404</v>
       </c>
-      <c r="J14" s="97">
+      <c r="J14" s="94">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="93"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="117"/>
       <c r="H15" s="65" t="s">
         <v>410</v>
       </c>
-      <c r="I15" s="95"/>
-      <c r="J15" s="98"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="95"/>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="99">
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="96">
         <v>0.38</v>
       </c>
       <c r="H16" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="I16" s="101" t="s">
+      <c r="I16" s="98" t="s">
         <v>404</v>
       </c>
-      <c r="J16" s="103">
+      <c r="J16" s="100">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="100"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="97"/>
       <c r="H17" s="60" t="s">
         <v>410</v>
       </c>
-      <c r="I17" s="102"/>
-      <c r="J17" s="104"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="101"/>
     </row>
     <row r="18" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="88"/>
-      <c r="E18" s="89"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="76"/>
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
@@ -7562,8 +7597,8 @@
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="88"/>
-      <c r="E19" s="92"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="78"/>
       <c r="F19" s="33" t="s">
         <v>411</v>
       </c>
@@ -7581,7 +7616,7 @@
       </c>
     </row>
     <row r="20" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="89"/>
+      <c r="D20" s="76"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -7590,57 +7625,57 @@
       <c r="J20" s="29"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D21" s="88"/>
-      <c r="E21" s="91" t="s">
+      <c r="D21" s="115"/>
+      <c r="E21" s="75" t="s">
         <v>412</v>
       </c>
-      <c r="F21" s="105" t="s">
+      <c r="F21" s="102" t="s">
         <v>413</v>
       </c>
       <c r="G21" s="26">
         <v>0.25</v>
       </c>
-      <c r="H21" s="96" t="s">
+      <c r="H21" s="105" t="s">
         <v>414</v>
       </c>
-      <c r="I21" s="96"/>
+      <c r="I21" s="105"/>
       <c r="J21" s="28">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D22" s="88"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="106"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="103"/>
       <c r="G22" s="58">
         <v>0.35</v>
       </c>
-      <c r="H22" s="108" t="s">
+      <c r="H22" s="106" t="s">
         <v>414</v>
       </c>
-      <c r="I22" s="108"/>
+      <c r="I22" s="106"/>
       <c r="J22" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="88"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="107"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="104"/>
       <c r="G23" s="71">
         <v>0.38</v>
       </c>
-      <c r="H23" s="109" t="s">
+      <c r="H23" s="107" t="s">
         <v>414</v>
       </c>
-      <c r="I23" s="109"/>
+      <c r="I23" s="107"/>
       <c r="J23" s="38">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="88"/>
-      <c r="E24" s="89"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="76"/>
       <c r="F24" s="39"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
@@ -7648,33 +7683,33 @@
       <c r="J24" s="40"/>
     </row>
     <row r="25" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="88"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="105" t="s">
+      <c r="D25" s="115"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="102" t="s">
         <v>415</v>
       </c>
       <c r="G25" s="26">
         <v>0.35</v>
       </c>
-      <c r="H25" s="96" t="s">
+      <c r="H25" s="105" t="s">
         <v>414</v>
       </c>
-      <c r="I25" s="96"/>
+      <c r="I25" s="105"/>
       <c r="J25" s="28">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="90"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="107"/>
+      <c r="D26" s="116"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="104"/>
       <c r="G26" s="71">
         <v>0.38</v>
       </c>
-      <c r="H26" s="109" t="s">
+      <c r="H26" s="107" t="s">
         <v>414</v>
       </c>
-      <c r="I26" s="109"/>
+      <c r="I26" s="107"/>
       <c r="J26" s="38">
         <v>14</v>
       </c>
@@ -7689,55 +7724,55 @@
       <c r="J27" s="16"/>
     </row>
     <row r="28" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="91" t="s">
+      <c r="D28" s="75" t="s">
         <v>416</v>
       </c>
-      <c r="E28" s="91" t="s">
+      <c r="E28" s="75" t="s">
         <v>417</v>
       </c>
-      <c r="F28" s="111" t="s">
+      <c r="F28" s="79" t="s">
         <v>418</v>
       </c>
       <c r="G28" s="62">
         <v>0.25</v>
       </c>
-      <c r="H28" s="79" t="s">
+      <c r="H28" s="81" t="s">
         <v>414</v>
       </c>
-      <c r="I28" s="113"/>
+      <c r="I28" s="82"/>
       <c r="J28" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="110"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="77"/>
       <c r="G29" s="43">
         <v>0.35</v>
       </c>
-      <c r="H29" s="114"/>
-      <c r="I29" s="115"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="84"/>
       <c r="J29" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="112"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="80"/>
       <c r="G30" s="61">
         <v>0.38</v>
       </c>
-      <c r="H30" s="116"/>
-      <c r="I30" s="117"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="86"/>
       <c r="J30" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="89"/>
-      <c r="E31" s="110"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="77"/>
       <c r="F31" s="47"/>
       <c r="G31" s="48"/>
       <c r="H31" s="48"/>
@@ -7745,50 +7780,50 @@
       <c r="J31" s="49"/>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="111" t="s">
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="79" t="s">
         <v>415</v>
       </c>
       <c r="G32" s="62">
         <v>0.25</v>
       </c>
-      <c r="H32" s="79" t="s">
+      <c r="H32" s="81" t="s">
         <v>419</v>
       </c>
-      <c r="I32" s="113"/>
+      <c r="I32" s="82"/>
       <c r="J32" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="110"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="77"/>
       <c r="G33" s="43">
         <v>0.35</v>
       </c>
-      <c r="H33" s="114"/>
-      <c r="I33" s="115"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="84"/>
       <c r="J33" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="89"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="112"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="80"/>
       <c r="G34" s="61">
         <v>0.38</v>
       </c>
-      <c r="H34" s="116"/>
-      <c r="I34" s="117"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="86"/>
       <c r="J34" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D35" s="110"/>
+      <c r="D35" s="77"/>
       <c r="E35" s="47"/>
       <c r="F35" s="47"/>
       <c r="G35" s="48"/>
@@ -7797,53 +7832,53 @@
       <c r="J35" s="49"/>
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D36" s="89"/>
-      <c r="E36" s="91" t="s">
+      <c r="D36" s="76"/>
+      <c r="E36" s="75" t="s">
         <v>420</v>
       </c>
-      <c r="F36" s="111" t="s">
+      <c r="F36" s="79" t="s">
         <v>421</v>
       </c>
       <c r="G36" s="62">
         <v>0.25</v>
       </c>
-      <c r="H36" s="79" t="s">
+      <c r="H36" s="81" t="s">
         <v>404</v>
       </c>
-      <c r="I36" s="113"/>
+      <c r="I36" s="82"/>
       <c r="J36" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D37" s="89"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="110"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="77"/>
       <c r="G37" s="43">
         <v>0.35</v>
       </c>
-      <c r="H37" s="114"/>
-      <c r="I37" s="115"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="84"/>
       <c r="J37" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D38" s="89"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="112"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="80"/>
       <c r="G38" s="61">
         <v>0.38</v>
       </c>
-      <c r="H38" s="116"/>
-      <c r="I38" s="117"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="86"/>
       <c r="J38" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="89"/>
-      <c r="E39" s="110"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="77"/>
       <c r="F39" s="47"/>
       <c r="G39" s="48"/>
       <c r="H39" s="48"/>
@@ -7851,51 +7886,51 @@
       <c r="J39" s="49"/>
     </row>
     <row r="40" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D40" s="89"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="111" t="s">
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="79" t="s">
         <v>422</v>
       </c>
       <c r="G40" s="62">
         <v>0.25</v>
       </c>
-      <c r="H40" s="79" t="s">
+      <c r="H40" s="81" t="s">
         <v>404</v>
       </c>
-      <c r="I40" s="113"/>
+      <c r="I40" s="82"/>
       <c r="J40" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="110"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="77"/>
       <c r="G41" s="43">
         <v>0.35</v>
       </c>
-      <c r="H41" s="114"/>
-      <c r="I41" s="115"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="84"/>
       <c r="J41" s="44">
         <v>14</v>
       </c>
       <c r="O41" s="50"/>
     </row>
     <row r="42" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="89"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="112"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="80"/>
       <c r="G42" s="61">
         <v>0.38</v>
       </c>
-      <c r="H42" s="116"/>
-      <c r="I42" s="117"/>
+      <c r="H42" s="85"/>
+      <c r="I42" s="86"/>
       <c r="J42" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D43" s="110"/>
+      <c r="D43" s="77"/>
       <c r="E43" s="47"/>
       <c r="F43" s="47"/>
       <c r="G43" s="48"/>
@@ -7904,33 +7939,33 @@
       <c r="J43" s="49"/>
     </row>
     <row r="44" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D44" s="89"/>
-      <c r="E44" s="111" t="s">
+      <c r="D44" s="76"/>
+      <c r="E44" s="79" t="s">
         <v>423</v>
       </c>
-      <c r="F44" s="118" t="s">
+      <c r="F44" s="87" t="s">
         <v>424</v>
       </c>
       <c r="G44" s="41">
         <v>0.25</v>
       </c>
-      <c r="H44" s="79" t="s">
+      <c r="H44" s="81" t="s">
         <v>425</v>
       </c>
-      <c r="I44" s="80"/>
+      <c r="I44" s="89"/>
       <c r="J44" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D45" s="92"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="119"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="88"/>
       <c r="G45" s="45">
         <v>0.38</v>
       </c>
-      <c r="H45" s="81"/>
-      <c r="I45" s="82"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="91"/>
       <c r="J45" s="46">
         <v>1</v>
       </c>
@@ -7945,55 +7980,55 @@
       <c r="J46" s="53"/>
     </row>
     <row r="47" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="91" t="s">
+      <c r="D47" s="75" t="s">
         <v>426</v>
       </c>
-      <c r="E47" s="91" t="s">
+      <c r="E47" s="75" t="s">
         <v>417</v>
       </c>
-      <c r="F47" s="111" t="s">
+      <c r="F47" s="79" t="s">
         <v>418</v>
       </c>
       <c r="G47" s="62">
         <v>0.25</v>
       </c>
-      <c r="H47" s="79" t="s">
+      <c r="H47" s="81" t="s">
         <v>419</v>
       </c>
-      <c r="I47" s="113"/>
+      <c r="I47" s="82"/>
       <c r="J47" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="48" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="110"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="77"/>
       <c r="G48" s="43">
         <v>0.35</v>
       </c>
-      <c r="H48" s="114"/>
-      <c r="I48" s="115"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="84"/>
       <c r="J48" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="89"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="112"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="80"/>
       <c r="G49" s="61">
         <v>0.38</v>
       </c>
-      <c r="H49" s="116"/>
-      <c r="I49" s="117"/>
+      <c r="H49" s="85"/>
+      <c r="I49" s="86"/>
       <c r="J49" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D50" s="89"/>
-      <c r="E50" s="110"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="77"/>
       <c r="F50" s="47"/>
       <c r="G50" s="48"/>
       <c r="H50" s="48"/>
@@ -8001,50 +8036,50 @@
       <c r="J50" s="49"/>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D51" s="89"/>
-      <c r="E51" s="89"/>
-      <c r="F51" s="111" t="s">
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="79" t="s">
         <v>415</v>
       </c>
       <c r="G51" s="62">
         <v>0.25</v>
       </c>
-      <c r="H51" s="79" t="s">
+      <c r="H51" s="81" t="s">
         <v>419</v>
       </c>
-      <c r="I51" s="113"/>
+      <c r="I51" s="82"/>
       <c r="J51" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D52" s="89"/>
-      <c r="E52" s="89"/>
-      <c r="F52" s="110"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="77"/>
       <c r="G52" s="43">
         <v>0.35</v>
       </c>
-      <c r="H52" s="114"/>
-      <c r="I52" s="115"/>
+      <c r="H52" s="83"/>
+      <c r="I52" s="84"/>
       <c r="J52" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D53" s="89"/>
-      <c r="E53" s="92"/>
-      <c r="F53" s="112"/>
+      <c r="D53" s="76"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="80"/>
       <c r="G53" s="61">
         <v>0.38</v>
       </c>
-      <c r="H53" s="116"/>
-      <c r="I53" s="117"/>
+      <c r="H53" s="85"/>
+      <c r="I53" s="86"/>
       <c r="J53" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="54" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="110"/>
+      <c r="D54" s="77"/>
       <c r="E54" s="47"/>
       <c r="F54" s="47"/>
       <c r="G54" s="48"/>
@@ -8053,53 +8088,53 @@
       <c r="J54" s="49"/>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D55" s="89"/>
-      <c r="E55" s="91" t="s">
+      <c r="D55" s="76"/>
+      <c r="E55" s="75" t="s">
         <v>420</v>
       </c>
-      <c r="F55" s="111" t="s">
+      <c r="F55" s="79" t="s">
         <v>421</v>
       </c>
       <c r="G55" s="62">
         <v>0.25</v>
       </c>
-      <c r="H55" s="79" t="s">
+      <c r="H55" s="81" t="s">
         <v>404</v>
       </c>
-      <c r="I55" s="80"/>
+      <c r="I55" s="89"/>
       <c r="J55" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D56" s="89"/>
-      <c r="E56" s="89"/>
-      <c r="F56" s="110"/>
+      <c r="D56" s="76"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="77"/>
       <c r="G56" s="43">
         <v>0.35</v>
       </c>
-      <c r="H56" s="120"/>
-      <c r="I56" s="121"/>
+      <c r="H56" s="92"/>
+      <c r="I56" s="93"/>
       <c r="J56" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="57" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D57" s="89"/>
-      <c r="E57" s="89"/>
-      <c r="F57" s="112"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="80"/>
       <c r="G57" s="61">
         <v>0.38</v>
       </c>
-      <c r="H57" s="81"/>
-      <c r="I57" s="82"/>
+      <c r="H57" s="90"/>
+      <c r="I57" s="91"/>
       <c r="J57" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="58" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D58" s="89"/>
-      <c r="E58" s="110"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="77"/>
       <c r="F58" s="47"/>
       <c r="G58" s="48"/>
       <c r="H58" s="48"/>
@@ -8107,50 +8142,50 @@
       <c r="J58" s="49"/>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D59" s="89"/>
-      <c r="E59" s="89"/>
-      <c r="F59" s="111" t="s">
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="79" t="s">
         <v>427</v>
       </c>
       <c r="G59" s="62">
         <v>0.25</v>
       </c>
-      <c r="H59" s="79" t="s">
+      <c r="H59" s="81" t="s">
         <v>404</v>
       </c>
-      <c r="I59" s="80"/>
+      <c r="I59" s="89"/>
       <c r="J59" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D60" s="89"/>
-      <c r="E60" s="89"/>
-      <c r="F60" s="110"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="77"/>
       <c r="G60" s="43">
         <v>0.35</v>
       </c>
-      <c r="H60" s="120"/>
-      <c r="I60" s="121"/>
+      <c r="H60" s="92"/>
+      <c r="I60" s="93"/>
       <c r="J60" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D61" s="89"/>
-      <c r="E61" s="92"/>
-      <c r="F61" s="112"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="78"/>
+      <c r="F61" s="80"/>
       <c r="G61" s="61">
         <v>0.38</v>
       </c>
-      <c r="H61" s="81"/>
-      <c r="I61" s="82"/>
+      <c r="H61" s="90"/>
+      <c r="I61" s="91"/>
       <c r="J61" s="46">
         <v>14</v>
       </c>
     </row>
     <row r="62" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D62" s="89"/>
+      <c r="D62" s="76"/>
       <c r="E62" s="54"/>
       <c r="F62" s="47"/>
       <c r="G62" s="48"/>
@@ -8159,33 +8194,33 @@
       <c r="J62" s="49"/>
     </row>
     <row r="63" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D63" s="89"/>
-      <c r="E63" s="111" t="s">
+      <c r="D63" s="76"/>
+      <c r="E63" s="79" t="s">
         <v>423</v>
       </c>
-      <c r="F63" s="118" t="s">
+      <c r="F63" s="87" t="s">
         <v>424</v>
       </c>
       <c r="G63" s="62">
         <v>0.25</v>
       </c>
-      <c r="H63" s="79" t="s">
+      <c r="H63" s="81" t="s">
         <v>425</v>
       </c>
-      <c r="I63" s="80"/>
+      <c r="I63" s="89"/>
       <c r="J63" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D64" s="92"/>
-      <c r="E64" s="112"/>
-      <c r="F64" s="119"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="80"/>
+      <c r="F64" s="88"/>
       <c r="G64" s="61">
         <v>0.38</v>
       </c>
-      <c r="H64" s="81"/>
-      <c r="I64" s="82"/>
+      <c r="H64" s="90"/>
+      <c r="I64" s="91"/>
       <c r="J64" s="46">
         <v>1</v>
       </c>
@@ -8207,6 +8242,47 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D11:D26"/>
+    <mergeCell ref="E11:E19"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D28:D45"/>
+    <mergeCell ref="E28:E34"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="H28:I30"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="H32:I34"/>
+    <mergeCell ref="E36:E42"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="H36:I38"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="H40:I42"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="H44:I45"/>
     <mergeCell ref="D47:D64"/>
     <mergeCell ref="E47:E53"/>
     <mergeCell ref="F47:F49"/>
@@ -8221,47 +8297,6 @@
     <mergeCell ref="H55:I57"/>
     <mergeCell ref="F59:F61"/>
     <mergeCell ref="H59:I61"/>
-    <mergeCell ref="D28:D45"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="H28:I30"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="H32:I34"/>
-    <mergeCell ref="E36:E42"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="H36:I38"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="H40:I42"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="H44:I45"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D11:D26"/>
-    <mergeCell ref="E11:E19"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11932,31 +11967,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C35"/>
+  <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
     <col min="3" max="3" width="77.109375" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>126</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>127</v>
       </c>
@@ -11966,8 +12002,11 @@
       <c r="C4" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="122" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>130</v>
       </c>
@@ -11978,7 +12017,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>133</v>
       </c>
@@ -11989,7 +12028,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>135</v>
       </c>
@@ -12000,7 +12039,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>137</v>
       </c>
@@ -12011,7 +12050,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>140</v>
       </c>
@@ -12022,7 +12061,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>142</v>
       </c>
@@ -12033,7 +12072,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="16.8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>144</v>
       </c>
@@ -12044,7 +12083,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>146</v>
       </c>
@@ -12054,8 +12093,11 @@
       <c r="C12" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="123" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>148</v>
       </c>
@@ -12065,8 +12107,11 @@
       <c r="C13" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D13" s="123" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>150</v>
       </c>
@@ -12076,8 +12121,11 @@
       <c r="C14" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D14" s="123" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>152</v>
       </c>
@@ -12087,8 +12135,11 @@
       <c r="C15" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>154</v>
       </c>
@@ -12099,7 +12150,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>157</v>
       </c>
@@ -12110,7 +12161,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>159</v>
       </c>
@@ -12121,7 +12172,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>161</v>
       </c>
@@ -12132,7 +12183,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>164</v>
       </c>
@@ -12143,7 +12194,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>166</v>
       </c>
@@ -12154,7 +12205,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>168</v>
       </c>
@@ -12164,8 +12215,11 @@
       <c r="C22" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>170</v>
       </c>
@@ -12175,8 +12229,11 @@
       <c r="C23" s="4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>172</v>
       </c>
@@ -12186,8 +12243,11 @@
       <c r="C24" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>174</v>
       </c>
@@ -12197,8 +12257,11 @@
       <c r="C25" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D25" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>176</v>
       </c>
@@ -12208,8 +12271,11 @@
       <c r="C26" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D26" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>178</v>
       </c>
@@ -12219,8 +12285,11 @@
       <c r="C27" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D27" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>180</v>
       </c>
@@ -12230,8 +12299,11 @@
       <c r="C28" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="124" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>182</v>
       </c>
@@ -12241,8 +12313,11 @@
       <c r="C29" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>184</v>
       </c>
@@ -12252,8 +12327,11 @@
       <c r="C30" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>186</v>
       </c>
@@ -12263,8 +12341,11 @@
       <c r="C31" s="4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>188</v>
       </c>
@@ -12274,8 +12355,11 @@
       <c r="C32" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>190</v>
       </c>
@@ -12285,8 +12369,11 @@
       <c r="C33" s="4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>192</v>
       </c>
@@ -12296,8 +12383,11 @@
       <c r="C34" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>194</v>
       </c>
@@ -12307,8 +12397,17 @@
       <c r="C35" s="4" t="s">
         <v>195</v>
       </c>
+      <c r="D35" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>502</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>